<commit_message>
test categorie EG 1c310f44a1d7379ea7e00f0f2916caa3f6713de1
</commit_message>
<xml_diff>
--- a/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
+++ b/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="473">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-01T16:42:37+00:00</t>
+    <t>2024-02-01T17:08:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -973,7 +973,7 @@
 </t>
   </si>
   <si>
-    <t>Concept that represents the overall questionnaire</t>
+    <t>Catégorie(s) d'EG pour lesquelles cette fiche de consigne de saisie est disponible</t>
   </si>
   <si>
     <t>An identifier for this question or group of questions in a particular terminology such as LOINC.</t>
@@ -985,13 +985,7 @@
     <t>Allows linking of the complete Questionnaire resources to formal terminologies.  It's common for "panels" of questions to be identified by a code.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes for questionnaires, groups and individual questions.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/questionnaire-questions</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J55-CategorieEG-ROR/FHIR/JDV-J55-CategorieEG-ROR</t>
   </si>
   <si>
     <t>.code</t>
@@ -1121,6 +1115,15 @@
   </si>
   <si>
     <t>Allows linking of groups of questions to formal terminologies.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes for questionnaires, groups and individual questions.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/questionnaire-questions</t>
   </si>
   <si>
     <t>Questionnaire.item.prefix</t>
@@ -1846,7 +1849,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="86.3125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.6953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="83.44921875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -5415,10 +5418,10 @@
         <v>78</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>80</v>
@@ -5464,13 +5467,11 @@
         <v>80</v>
       </c>
       <c r="X31" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="Y31" s="2"/>
+      <c r="Z31" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="Z31" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>80</v>
@@ -5506,7 +5507,7 @@
         <v>80</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>80</v>
@@ -5515,15 +5516,15 @@
         <v>80</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5546,16 +5547,16 @@
         <v>80</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="M32" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -5605,7 +5606,7 @@
         <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5614,16 +5615,16 @@
         <v>79</v>
       </c>
       <c r="AI32" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL32" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>80</v>
@@ -5637,10 +5638,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5666,10 +5667,10 @@
         <v>168</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5720,7 +5721,7 @@
         <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5752,10 +5753,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5784,7 +5785,7 @@
         <v>136</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>138</v>
@@ -5837,7 +5838,7 @@
         <v>141</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
@@ -5869,14 +5870,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5898,10 +5899,10 @@
         <v>135</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>138</v>
@@ -5956,7 +5957,7 @@
         <v>80</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5988,10 +5989,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6017,16 +6018,16 @@
         <v>168</v>
       </c>
       <c r="L36" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="N36" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="O36" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="O36" t="s" s="2">
-        <v>340</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>80</v>
@@ -6075,7 +6076,7 @@
         <v>80</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>87</v>
@@ -6093,7 +6094,7 @@
         <v>80</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>80</v>
@@ -6107,10 +6108,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6136,16 +6137,16 @@
         <v>103</v>
       </c>
       <c r="L37" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="N37" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="O37" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>80</v>
@@ -6194,7 +6195,7 @@
         <v>80</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -6212,7 +6213,7 @@
         <v>80</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>80</v>
@@ -6226,10 +6227,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6255,16 +6256,16 @@
         <v>306</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="N38" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="O38" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>80</v>
@@ -6289,13 +6290,13 @@
         <v>80</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>312</v>
+        <v>352</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>313</v>
+        <v>353</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>80</v>
@@ -6313,7 +6314,7 @@
         <v>80</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6322,7 +6323,7 @@
         <v>79</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>100</v>
@@ -6331,7 +6332,7 @@
         <v>80</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>80</v>
@@ -6340,19 +6341,19 @@
         <v>80</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6374,16 +6375,16 @@
         <v>168</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>80</v>
@@ -6432,7 +6433,7 @@
         <v>80</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6450,7 +6451,7 @@
         <v>80</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>80</v>
@@ -6464,10 +6465,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6493,13 +6494,13 @@
         <v>168</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6549,7 +6550,7 @@
         <v>80</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6581,10 +6582,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6610,16 +6611,16 @@
         <v>110</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>80</v>
@@ -6647,10 +6648,10 @@
         <v>199</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>80</v>
@@ -6668,7 +6669,7 @@
         <v>80</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>87</v>
@@ -6686,7 +6687,7 @@
         <v>80</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>80</v>
@@ -6700,10 +6701,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6726,19 +6727,19 @@
         <v>80</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>80</v>
@@ -6787,7 +6788,7 @@
         <v>80</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6799,13 +6800,13 @@
         <v>99</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>80</v>
@@ -6819,10 +6820,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6848,10 +6849,10 @@
         <v>168</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6902,7 +6903,7 @@
         <v>80</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6934,10 +6935,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6966,7 +6967,7 @@
         <v>136</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N44" t="s" s="2">
         <v>138</v>
@@ -7019,7 +7020,7 @@
         <v>141</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -7051,14 +7052,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7080,10 +7081,10 @@
         <v>135</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>138</v>
@@ -7138,7 +7139,7 @@
         <v>80</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -7170,10 +7171,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7199,13 +7200,13 @@
         <v>168</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7255,7 +7256,7 @@
         <v>80</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>87</v>
@@ -7273,7 +7274,7 @@
         <v>80</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>80</v>
@@ -7287,10 +7288,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7316,13 +7317,13 @@
         <v>110</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7351,10 +7352,10 @@
         <v>199</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>80</v>
@@ -7372,7 +7373,7 @@
         <v>80</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>87</v>
@@ -7390,7 +7391,7 @@
         <v>80</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>80</v>
@@ -7404,10 +7405,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7430,13 +7431,13 @@
         <v>80</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7463,13 +7464,13 @@
         <v>80</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>80</v>
@@ -7487,7 +7488,7 @@
         <v>80</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>87</v>
@@ -7496,7 +7497,7 @@
         <v>87</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>100</v>
@@ -7505,7 +7506,7 @@
         <v>80</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>80</v>
@@ -7519,10 +7520,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7548,13 +7549,13 @@
         <v>110</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7583,10 +7584,10 @@
         <v>199</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>80</v>
@@ -7604,7 +7605,7 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7613,7 +7614,7 @@
         <v>87</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>100</v>
@@ -7622,7 +7623,7 @@
         <v>80</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>80</v>
@@ -7636,10 +7637,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7665,20 +7666,20 @@
         <v>206</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q50" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="R50" t="s" s="2">
         <v>80</v>
@@ -7723,7 +7724,7 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7732,7 +7733,7 @@
         <v>87</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>100</v>
@@ -7741,7 +7742,7 @@
         <v>80</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>80</v>
@@ -7755,10 +7756,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7784,76 +7785,76 @@
         <v>206</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="P51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q51" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF51" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="M51" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="P51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Q51" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="R51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AF51" t="s" s="2">
+      <c r="AG51" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI51" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>100</v>
@@ -7862,7 +7863,7 @@
         <v>80</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>80</v>
@@ -7876,10 +7877,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7905,16 +7906,16 @@
         <v>206</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>80</v>
@@ -7963,7 +7964,7 @@
         <v>80</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
@@ -7972,7 +7973,7 @@
         <v>87</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>100</v>
@@ -7981,7 +7982,7 @@
         <v>80</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>80</v>
@@ -7995,10 +7996,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8021,16 +8022,16 @@
         <v>80</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -8080,7 +8081,7 @@
         <v>80</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>78</v>
@@ -8089,7 +8090,7 @@
         <v>87</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>100</v>
@@ -8098,7 +8099,7 @@
         <v>80</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>80</v>
@@ -8112,10 +8113,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8138,16 +8139,16 @@
         <v>80</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8197,7 +8198,7 @@
         <v>80</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>78</v>
@@ -8206,7 +8207,7 @@
         <v>87</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>100</v>
@@ -8215,7 +8216,7 @@
         <v>80</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>80</v>
@@ -8229,10 +8230,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8255,16 +8256,16 @@
         <v>80</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8314,7 +8315,7 @@
         <v>80</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
@@ -8323,7 +8324,7 @@
         <v>79</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>100</v>
@@ -8332,7 +8333,7 @@
         <v>80</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>80</v>
@@ -8346,10 +8347,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8375,10 +8376,10 @@
         <v>168</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8429,7 +8430,7 @@
         <v>80</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>78</v>
@@ -8461,10 +8462,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8493,7 +8494,7 @@
         <v>136</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>138</v>
@@ -8546,7 +8547,7 @@
         <v>141</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8578,14 +8579,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -8607,10 +8608,10 @@
         <v>135</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>138</v>
@@ -8665,7 +8666,7 @@
         <v>80</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
@@ -8697,10 +8698,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8723,16 +8724,16 @@
         <v>80</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
@@ -8758,13 +8759,13 @@
         <v>80</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>80</v>
@@ -8782,7 +8783,7 @@
         <v>80</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>87</v>
@@ -8800,7 +8801,7 @@
         <v>80</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>80</v>
@@ -8814,10 +8815,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8843,20 +8844,20 @@
         <v>206</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q60" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R60" t="s" s="2">
         <v>80</v>
@@ -8901,7 +8902,7 @@
         <v>80</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>78</v>
@@ -8919,7 +8920,7 @@
         <v>80</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>80</v>
@@ -8933,10 +8934,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8959,19 +8960,19 @@
         <v>80</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O61" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>80</v>
@@ -9020,7 +9021,7 @@
         <v>80</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>78</v>
@@ -9029,7 +9030,7 @@
         <v>79</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>100</v>
@@ -9038,7 +9039,7 @@
         <v>80</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>80</v>
@@ -9052,10 +9053,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9081,10 +9082,10 @@
         <v>168</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -9135,7 +9136,7 @@
         <v>80</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>78</v>
@@ -9167,10 +9168,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9199,7 +9200,7 @@
         <v>136</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N63" t="s" s="2">
         <v>138</v>
@@ -9252,7 +9253,7 @@
         <v>141</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>78</v>
@@ -9284,14 +9285,14 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
@@ -9313,10 +9314,10 @@
         <v>135</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N64" t="s" s="2">
         <v>138</v>
@@ -9371,7 +9372,7 @@
         <v>80</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>78</v>
@@ -9403,10 +9404,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9429,16 +9430,16 @@
         <v>80</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9464,13 +9465,13 @@
         <v>80</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="Z65" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AA65" t="s" s="2">
         <v>80</v>
@@ -9488,7 +9489,7 @@
         <v>80</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>87</v>
@@ -9506,7 +9507,7 @@
         <v>80</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>80</v>
@@ -9520,10 +9521,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9549,16 +9550,16 @@
         <v>81</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O66" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P66" t="s" s="2">
         <v>80</v>
@@ -9607,7 +9608,7 @@
         <v>80</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>78</v>
@@ -9616,7 +9617,7 @@
         <v>79</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>80</v>
@@ -9625,7 +9626,7 @@
         <v>80</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
modifications suite demandes ROR 80a7af4f89704016607bb968b5df8b68dbcb5f08
</commit_message>
<xml_diff>
--- a/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
+++ b/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-01T17:43:36+00:00</t>
+    <t>2024-02-01T18:39:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -607,7 +607,7 @@
 </t>
   </si>
   <si>
-    <t>Instantiates protocol or definition</t>
+    <t>Fiche(s) de saisie source</t>
   </si>
   <si>
     <t>The URL of a Questionnaire that this Questionnaire is based on.</t>
@@ -3652,7 +3652,7 @@
         <v>79</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
ajout code categorieEG d0ad72fe73c161c02ce3c9b0acd8fd2766c6ab89
</commit_message>
<xml_diff>
--- a/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
+++ b/ig/sd-questionnaire/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-01T18:39:39+00:00</t>
+    <t>2024-02-02T08:32:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -607,7 +607,7 @@
 </t>
   </si>
   <si>
-    <t>Fiche(s) de saisie source</t>
+    <t>Fiche(s) de saisie parente(s)</t>
   </si>
   <si>
     <t>The URL of a Questionnaire that this Questionnaire is based on.</t>
@@ -5415,7 +5415,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>79</v>

</xml_diff>